<commit_message>
new matrix distance possibility
</commit_message>
<xml_diff>
--- a/IOTSCv2.xlsx
+++ b/IOTSCv2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="14810" windowHeight="8010"/>
+    <workbookView activeTab="0" windowWidth="19200" windowHeight="8090"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,17 @@
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <webPublishing allowPng="1" css="0" codePage="1252"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2" count="2">
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>coordinates</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58,20 +69,20 @@
       <b val="0"/>
       <i val="0"/>
       <u val="none"/>
-      <color rgb="FF444444"/>
-      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <vertAlign val="baseline"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <strike val="0"/>
     </font>
     <font>
       <b val="0"/>
       <i val="0"/>
       <u val="none"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
       <vertAlign val="baseline"/>
-      <sz val="10"/>
+      <sz val="11"/>
       <strike val="0"/>
     </font>
   </fonts>
@@ -209,7 +220,7 @@
       <protection locked="1" hidden="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
@@ -230,35 +241,31 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="0" borderId="4" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="0" borderId="5" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="0" borderId="5" numFmtId="10" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="0" borderId="0" numFmtId="100" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="0" borderId="6" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="0" borderId="7" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="0" borderId="7" numFmtId="10" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="0" borderId="4" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="0" borderId="5" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="0" borderId="5" numFmtId="10" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="0" borderId="0" numFmtId="100" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="0" borderId="6" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="0" borderId="7" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="0" borderId="7" numFmtId="10" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
     </xf>
@@ -274,7 +281,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -283,7 +290,8 @@
     <col min="3" max="3" style="1" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" style="1" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" style="1" width="24.425781249999996" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" style="1" width="9.142307692307693"/>
+    <col min="6" max="6" style="1" width="12.99921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" style="1" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
@@ -304,90 +312,110 @@
       </c>
       <c r="D1" s="4" t="inlineStr">
         <is>
-          <t>Location (Latitude)</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>Location (Longitude)</t>
-        </is>
-      </c>
-      <c r="F1" s="5"/>
+          <t>latitude</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Evolua Mercado Sustentavel</t>
         </is>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>0.96250000000000002</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>-15.760026399999999</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>-47.882887400000001</v>
+      </c>
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>-15.7600264,-47.8828874</t>
+        </is>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>Sede Green Ambiental</t>
         </is>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>0.96879999999999999</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>-15.795753899999999</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>-47.988937999999997</v>
+      </c>
+      <c r="F3" s="0" t="inlineStr">
+        <is>
+          <t>-15.7957539,-47.988938</t>
+        </is>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>Dona de Casa</t>
         </is>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>0.84379999999999999</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>-15.768672199999999</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>-47.888866200000002</v>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>-15.7686722,-47.8888662</t>
+        </is>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="inlineStr">
+      <c r="B5" s="10" t="inlineStr">
         <is>
           <t>Esp Matheus</t>
         </is>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>0.5625</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>-15.7634302</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>-47.872481399999998</v>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>-15.7634302,-47.8724814</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 16 locations and tested
</commit_message>
<xml_diff>
--- a/IOTSCv2.xlsx
+++ b/IOTSCv2.xlsx
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2" count="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1" count="1">
   <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>coordinates</t>
+    <t>-15.8091836,-47.9001107</t>
   </si>
 </sst>
 </file>
@@ -278,15 +275,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A18" sqref="A18:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" style="1" width="9.142307692307693"/>
+    <col min="1" max="1" style="1" width="9.142307692307693"/>
+    <col min="2" max="2" style="1" width="74.1384014423077" bestFit="1" customWidth="1"/>
     <col min="3" max="3" style="1" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" style="1" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" style="1" width="24.425781249999996" bestFit="1" customWidth="1"/>
@@ -315,11 +313,15 @@
           <t>latitude</t>
         </is>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>1</v>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>longitude</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>coordinates</t>
+        </is>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -416,6 +418,292 @@
         <is>
           <t>-15.7634302,-47.8724814</t>
         </is>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Dona de Casa, Via W Tres Norte - Asa Norte, Brasilia - DF, 70297-400</t>
+        </is>
+      </c>
+      <c r="C6" s="7">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="D6" s="0">
+        <v>-15.7744312</v>
+      </c>
+      <c r="E6" s="0">
+        <v>-47.900262400000003</v>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>-15.7744312,-47.9002624</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>cobasi</t>
+        </is>
+      </c>
+      <c r="C7" s="7">
+        <v>0.96879999999999999</v>
+      </c>
+      <c r="D7" s="0">
+        <v>-15.736511399999999</v>
+      </c>
+      <c r="E7" s="0">
+        <v>-47.893102800000001</v>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>-15.7365114,-47.8931028</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>PÃ£o Dourado - Noroeste</t>
+        </is>
+      </c>
+      <c r="C8" s="7">
+        <v>0.84379999999999999</v>
+      </c>
+      <c r="D8" s="0">
+        <v>-15.7408634</v>
+      </c>
+      <c r="E8" s="0">
+        <v>-47.9064549</v>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>-15.7408634,-47.9064549</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>Panificadora PÃ£o Prima</t>
+        </is>
+      </c>
+      <c r="C9" s="11">
+        <v>0.5625</v>
+      </c>
+      <c r="D9" s="0">
+        <v>-15.754970200000001</v>
+      </c>
+      <c r="E9" s="0">
+        <v>-47.898261599999998</v>
+      </c>
+      <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>-15.7549702,-47.8982616</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="0">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>Leroy Merlin Brasilia Norte, SOFN - Area Especial, Brasilia - DF, 70634-120</t>
+        </is>
+      </c>
+      <c r="C10" s="7">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="D10" s="0">
+        <v>-15.7525496</v>
+      </c>
+      <c r="E10" s="0">
+        <v>-47.930304499999998</v>
+      </c>
+      <c r="F10" s="0" t="inlineStr">
+        <is>
+          <t>-15.7525496,-47.9303045</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="0">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>Superquadra Norte 210 - Asa Norte, Brasilia - DF, 70862-000</t>
+        </is>
+      </c>
+      <c r="C11" s="7">
+        <v>0.96879999999999999</v>
+      </c>
+      <c r="D11" s="0">
+        <v>-15.755914199999999</v>
+      </c>
+      <c r="E11" s="0">
+        <v>-47.884851500000003</v>
+      </c>
+      <c r="F11" s="0" t="inlineStr">
+        <is>
+          <t>-15.7559142,-47.8848515</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>Superquadra Norte 115 - Asa Norte, Brasilia - DF, 70297-400</t>
+        </is>
+      </c>
+      <c r="C12" s="7">
+        <v>0.84379999999999999</v>
+      </c>
+      <c r="D12" s="0">
+        <v>-15.7416731</v>
+      </c>
+      <c r="E12" s="0">
+        <v>-47.893982000000001</v>
+      </c>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>-15.7416731,-47.893982</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="0">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>Administracao Regional de Lago Norte - St. De HabitaÃ§Ãµes Individuais Norte CA 5 - Lago Norte, Brasilia - DF, 71503-507</t>
+        </is>
+      </c>
+      <c r="C13" s="11">
+        <v>0.5625</v>
+      </c>
+      <c r="D13" s="0">
+        <v>-15.716620900000001</v>
+      </c>
+      <c r="E13" s="0">
+        <v>-47.885653499999997</v>
+      </c>
+      <c r="F13" s="0" t="inlineStr">
+        <is>
+          <t>-15.7166209,-47.8856535</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="27">
+      <c r="A14" s="0">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>PÃ£o de AÃ§Ãºcar - Sul 304/305</t>
+        </is>
+      </c>
+      <c r="C14" s="7">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="D14" s="0">
+        <v>-15.8040386</v>
+      </c>
+      <c r="E14" s="0">
+        <v>-47.894147099999998</v>
+      </c>
+      <c r="F14" s="0" t="inlineStr">
+        <is>
+          <t>-15.8040386,-47.8941471</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="0">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>Boteco do Juca</t>
+        </is>
+      </c>
+      <c r="C15" s="7">
+        <v>0.96879999999999999</v>
+      </c>
+      <c r="D15" s="0">
+        <v>-15.8090495</v>
+      </c>
+      <c r="E15" s="0">
+        <v>-47.893769499999998</v>
+      </c>
+      <c r="F15" s="0" t="inlineStr">
+        <is>
+          <t>-15.8090495,-47.8937695</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="27">
+      <c r="A16" s="0">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>Casa de Biscoitos Mineiros Asa Sul</t>
+        </is>
+      </c>
+      <c r="C16" s="7">
+        <v>0.84379999999999999</v>
+      </c>
+      <c r="D16" s="0">
+        <v>-15.809072199999999</v>
+      </c>
+      <c r="E16" s="0">
+        <v>-47.898075499999997</v>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
+        <is>
+          <t>-15.8090722,-47.8980755</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="27">
+      <c r="A17" s="0">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>Simpsons Asa Sul</t>
+        </is>
+      </c>
+      <c r="C17" s="11">
+        <v>0.5625</v>
+      </c>
+      <c r="D17" s="0">
+        <v>-15.809183600000001</v>
+      </c>
+      <c r="E17" s="0">
+        <v>-47.900110699999999</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>